<commit_message>
changed equals to equalsIgnoreCase for enum
</commit_message>
<xml_diff>
--- a/src/main/java/corecentra/qaqctool/storage/contribution_test.xlsx
+++ b/src/main/java/corecentra/qaqctool/storage/contribution_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\old project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E3BF7F-EBD4-4DF6-887A-2EC35320D32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402D5D34-EC64-4F08-AD19-3C164E816DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{CDE16FF3-6EE1-4F01-A311-4B428745FF28}"/>
   </bookViews>
@@ -494,7 +494,9 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>

</xml_diff>